<commit_message>
restructured files to be more modular
</commit_message>
<xml_diff>
--- a/VIP_results.xlsx
+++ b/VIP_results.xlsx
@@ -481,12 +481,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>https://www.instagram.com/barackobama/?hl=en</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>https://en.wikipedia.org/wiki/Barack_Obama</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/barackobama/?hl=en</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -516,14 +516,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>https://en.wikipedia.org/wiki/Elon_Musk</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>https://twitter.com/elonmusk</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Elon_Musk</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>https://www.tesla.com/elon-musk</t>
@@ -531,12 +531,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>https://www.spacex.com/</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>https://www.forbes.com/profile/elon-musk/</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>https://www.spacex.com/</t>
         </is>
       </c>
     </row>
@@ -631,17 +631,17 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>https://www.instagram.com/angelinajolie/p/CSzXXUHLzXt/</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://www.nytimes.com/2013/05/14/opinion/my-medical-choice.html</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>https://www.imdb.com/name/nm0001401/</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>https://www.nytimes.com/2013/05/14/opinion/my-medical-choice.html</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>https://www.cnn.com/2024/04/04/entertainment/angelina-jolie-brad-pitt-abuse-history/index.html</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>https://twitter.com/RobertDowneyJr</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>https://www.facebook.com/robertdowneyjr/</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>https://twitter.com/RobertDowneyJr</t>
         </is>
       </c>
     </row>
@@ -741,12 +741,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://people.com/tag/scarlett-johansson/</t>
+          <t>https://twitter.com/BobbyAllyn/status/1792679435701014908</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.hollywoodreporter.com/movies/movie-features/scarlett-johansson-talks-woody-allen-elizabeth-warren-black-widow-1235618/</t>
+          <t>https://www.bbc.com/news/articles/cm559l5g529o</t>
         </is>
       </c>
     </row>
@@ -761,22 +761,22 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>https://www.instagram.com/kanyewest/?hl=en</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>https://en.wikipedia.org/wiki/Kanye_West</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>https://twitter.com/kanyewest?lang=en</t>
-        </is>
-      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/kanyewest/?hl=en</t>
+          <t>https://www.youtube.com/channel/UCs6eXM7s8Vl5WcECcRHc2qQ</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/channel/UCs6eXM7s8Vl5WcECcRHc2qQ</t>
+          <t>https://www.youtube.com/watch?v=Tqlw87XV4kU</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -811,12 +811,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>https://www.linkedin.com/in/paul-jarrod-frank-md-1049682a</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>https://www.nytimes.com/2016/03/06/nyregion/how-paul-jarrod-frank-a-cosmeticdermatologist-spends-his-sundays.html</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/paul-jarrod-frank-md-1049682a</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
cleaned up log files
</commit_message>
<xml_diff>
--- a/VIP_results.xlsx
+++ b/VIP_results.xlsx
@@ -631,17 +631,17 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/angelinajolie/p/CSzXXUHLzXt/</t>
+          <t>https://www.nytimes.com/2013/05/14/opinion/my-medical-choice.html</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.nytimes.com/2013/05/14/opinion/my-medical-choice.html</t>
+          <t>https://www.imdb.com/name/nm0001401/</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.imdb.com/name/nm0001401/</t>
+          <t>https://www.bidmc.org/about-bidmc/blogs/living-with-cancer/2018/07/the-angelina-jolie-effect</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finished implementing basic UI
</commit_message>
<xml_diff>
--- a/VIP_results.xlsx
+++ b/VIP_results.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>VIP</t>
+          <t>VIP Status</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -481,14 +481,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>https://en.wikipedia.org/wiki/Barack_Obama</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>https://www.instagram.com/barackobama/?hl=en</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Barack_Obama</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>https://www.whitehouse.gov/about-the-white-house/presidents/barack-obama/</t>
@@ -501,7 +501,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://twitter.com/BarackObama</t>
+          <t>https://www.obamalibrary.gov/obamas/president-barack-obama</t>
         </is>
       </c>
     </row>
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -526,17 +526,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>https://www.forbes.com/profile/elon-musk/</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>https://www.tesla.com/elon-musk</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>https://www.spacex.com/</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>https://www.forbes.com/profile/elon-musk/</t>
         </is>
       </c>
     </row>
@@ -566,12 +566,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://twitter.com/Oprah</t>
+          <t>https://www.facebook.com/oprahwinfrey/</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/oprahwinfrey/</t>
+          <t>https://twitter.com/oprah</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/leonardodicaprio/</t>
+          <t>https://www.instagram.com/leonardodicaprio/?hl=en</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/p/Cgrw32FuiUN/?hl=en</t>
+          <t>https://www.instagram.com/p/CaWTsy5gwQY/?hl=en</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -666,12 +666,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>https://www.imdb.com/name/nm0000098/</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>https://www.instagram.com/p/Czq8K4DMOMQ/?hl=en</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>https://www.imdb.com/name/nm0000098/</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/robertdowneyjr/?hl=en</t>
+          <t>https://www.instagram.com/robertdowneyjr/</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -706,12 +706,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://twitter.com/RobertDowneyJr</t>
+          <t>https://www.facebook.com/robertdowneyjr/</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/robertdowneyjr/</t>
+          <t>https://twitter.com/robertdowneyjr</t>
         </is>
       </c>
     </row>
@@ -746,7 +746,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.bbc.com/news/articles/cm559l5g529o</t>
+          <t>https://www.nature.com/articles/d41586-024-01578-4</t>
         </is>
       </c>
     </row>
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>

</xml_diff>